<commit_message>
fix: multiple specs in service
</commit_message>
<xml_diff>
--- a/lucemData.xlsx
+++ b/lucemData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="523">
   <si>
     <t>Номер</t>
   </si>
@@ -128,7 +128,7 @@
   </si>
   <si>
     <t>2020 - 2022 НАО «Медицинский Университет Караганды», общая медицина, резидентура.||
-2018 - 2020 Карагандинский Государственный Медицинский Университет, Общая медицина, интернатура.||                                               
+2018 - 2020 Карагандинский Государственный Медицинский Университет, Общая медицина, интернатура.||                                        
 2013 - 2018 Карагандинский Государственный Медицинский Университет</t>
   </si>
   <si>
@@ -458,7 +458,7 @@
     <t>Кардиолог||Врач функциональной диагностики||Терапевт</t>
   </si>
   <si>
-    <t>1982-1988 ЦГМИ (Целиноградский Государственный Медицинский Институт)</t>
+    <t>1982 - 1988 ЦГМИ (Целиноградский Государственный Медицинский Институт)</t>
   </si>
   <si>
     <t>2016 - 2021 Клиническая электрокардиография, Неотложные вопросы терапии в кардиологии, Эхокардиография у пациентов с каларанной патологией.</t>
@@ -524,7 +524,7 @@
     <t>Кардиолог десткий||Педиатр||Врач функциональной диагностики</t>
   </si>
   <si>
-    <t>принимает только детей</t>
+    <t>Принимает только детей</t>
   </si>
   <si>
     <t xml:space="preserve">2006 - 2012 АО МУА бакалавриат по специальности педиатрия||
@@ -822,6 +822,9 @@
   </si>
   <si>
     <t>Детский Аллерголог||Педиатр</t>
+  </si>
+  <si>
+    <t>принимает только детей</t>
   </si>
   <si>
     <t>1979 - 1985 ЦГМИ, факультет педиатрии||
@@ -1157,7 +1160,7 @@
     <t>Тлеукабыловна</t>
   </si>
   <si>
-    <t>Акушер-гинеколог, Гинеколог</t>
+    <t>Акушер-гинеколог||Гинеколог</t>
   </si>
   <si>
     <t>Принимает дети и взрослых</t>
@@ -1320,9 +1323,6 @@
     <t>Вопрос</t>
   </si>
   <si>
-    <t>Гинеколог, Акушер-гинеколог</t>
-  </si>
-  <si>
     <t>Первичный осмотр</t>
   </si>
   <si>
@@ -1353,9 +1353,6 @@
     <t>Удаление ВМС в зав. от сложности</t>
   </si>
   <si>
-    <t>от 5000</t>
-  </si>
-  <si>
     <t>Лечение ИППП</t>
   </si>
   <si>
@@ -1377,9 +1374,6 @@
     <t>Удаление кандилом половых органов</t>
   </si>
   <si>
-    <t>от 2000</t>
-  </si>
-  <si>
     <t>Кардиолог</t>
   </si>
   <si>
@@ -1683,39 +1677,24 @@
     <t>удаление папиллом</t>
   </si>
   <si>
-    <t>от 1000</t>
-  </si>
-  <si>
     <t>удаление кандиллом</t>
   </si>
   <si>
     <t>удаление родинок</t>
   </si>
   <si>
-    <t>от 10000</t>
-  </si>
-  <si>
     <t>удаление малюсок</t>
   </si>
   <si>
-    <t>от 1200</t>
-  </si>
-  <si>
     <t>комбинированная чистка лица</t>
   </si>
   <si>
-    <t>от 9000</t>
-  </si>
-  <si>
     <t>поверхностый пилинг</t>
   </si>
   <si>
     <t>глубокий пилинг</t>
   </si>
   <si>
-    <t>от 8000</t>
-  </si>
-  <si>
     <t>мезотерапия лица</t>
   </si>
   <si>
@@ -1728,27 +1707,15 @@
     <t>аугментация (увеличение) губ</t>
   </si>
   <si>
-    <t>от 30000</t>
-  </si>
-  <si>
     <t>ботулинотерапия</t>
   </si>
   <si>
-    <t>от 15000</t>
-  </si>
-  <si>
     <t>лечение гипергидроза</t>
   </si>
   <si>
-    <t>от 40000</t>
-  </si>
-  <si>
     <t>плазмолифтинг лица</t>
   </si>
   <si>
-    <t>от 12000</t>
-  </si>
-  <si>
     <t>плазмолифтинг волос</t>
   </si>
   <si>
@@ -1758,9 +1725,6 @@
     <t>smas-lifting</t>
   </si>
   <si>
-    <t>от35000</t>
-  </si>
-  <si>
     <t>липофилинг (1 зона)</t>
   </si>
   <si>
@@ -1770,15 +1734,9 @@
     <t>липофилинг груди</t>
   </si>
   <si>
-    <t>от 250000</t>
-  </si>
-  <si>
     <t>липофилинг ягодиц</t>
   </si>
   <si>
-    <t>от 300000</t>
-  </si>
-  <si>
     <t>липофилинг рук</t>
   </si>
   <si>
@@ -1800,16 +1758,10 @@
     <t>лабиопластика</t>
   </si>
   <si>
-    <t>от 100000</t>
-  </si>
-  <si>
     <t>сужение влагалища smas</t>
   </si>
   <si>
     <t>лисьи глаза</t>
-  </si>
-  <si>
-    <t>от 60000</t>
   </si>
   <si>
     <t>липолитики</t>
@@ -2025,7 +1977,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2065,6 +2017,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
@@ -2843,7 +2798,7 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="9" t="s">
         <v>97</v>
       </c>
@@ -2873,7 +2828,7 @@
       <c r="E12" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G12" s="2"/>
@@ -3354,7 +3309,7 @@
         <v>201</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1">
@@ -3364,22 +3319,22 @@
         <v>37.0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -3412,16 +3367,16 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>130</v>
@@ -3434,10 +3389,10 @@
         <v>5.0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="4" t="s">
@@ -3458,13 +3413,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>52</v>
@@ -3478,13 +3433,13 @@
         <v>7.0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -3498,16 +3453,16 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>130</v>
@@ -3520,20 +3475,20 @@
         <v>6.0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>134</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -3544,16 +3499,16 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>130</v>
@@ -3567,15 +3522,15 @@
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -3586,16 +3541,16 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>130</v>
@@ -3608,13 +3563,13 @@
         <v>5.0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -3628,16 +3583,16 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>130</v>
@@ -3650,10 +3605,10 @@
         <v>21.0</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -3668,16 +3623,16 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>33</v>
@@ -3690,18 +3645,18 @@
         <v>5.0</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -3712,13 +3667,13 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>43</v>
@@ -3734,20 +3689,20 @@
         <v>5.0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -3758,16 +3713,16 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>33</v>
@@ -3780,22 +3735,22 @@
         <v>13.0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
@@ -3806,16 +3761,16 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>22</v>
@@ -3846,19 +3801,19 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1">
@@ -3868,20 +3823,20 @@
         <v>13.0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>134</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -3892,16 +3847,16 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>33</v>
@@ -3915,13 +3870,13 @@
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -3932,22 +3887,22 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>130</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H37" s="1">
         <v>1987.0</v>
@@ -3956,16 +3911,16 @@
         <v>35.0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -3978,16 +3933,16 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>22</v>
@@ -4000,19 +3955,19 @@
         <v>6.0</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -4024,16 +3979,16 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>130</v>
@@ -4046,20 +4001,20 @@
         <v>13.0</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>159</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
@@ -5491,25 +5446,25 @@
   <sheetData>
     <row r="1" ht="81.0" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -5517,8 +5472,8 @@
       <c r="L1" s="11"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>324</v>
+      <c r="A2" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>325</v>
@@ -5539,8 +5494,8 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>324</v>
+      <c r="A3" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>327</v>
@@ -5561,8 +5516,8 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>324</v>
+      <c r="A4" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>328</v>
@@ -5583,8 +5538,8 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>324</v>
+      <c r="A5" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>329</v>
@@ -5605,8 +5560,8 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>324</v>
+      <c r="A6" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>330</v>
@@ -5627,8 +5582,8 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>324</v>
+      <c r="A7" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>331</v>
@@ -5649,8 +5604,8 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>324</v>
+      <c r="A8" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>332</v>
@@ -5671,8 +5626,8 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>324</v>
+      <c r="A9" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>333</v>
@@ -5693,8 +5648,8 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>324</v>
+      <c r="A10" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>334</v>
@@ -5702,8 +5657,8 @@
       <c r="C10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>335</v>
+      <c r="D10" s="14">
+        <v>5000.0</v>
       </c>
       <c r="E10" s="1">
         <v>30.0</v>
@@ -5715,17 +5670,17 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>324</v>
+      <c r="A11" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>335</v>
+      <c r="D11" s="14">
+        <v>5000.0</v>
       </c>
       <c r="E11" s="1">
         <v>30.0</v>
@@ -5737,11 +5692,11 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>324</v>
+      <c r="A12" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>48</v>
@@ -5759,11 +5714,11 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>324</v>
+      <c r="A13" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>48</v>
@@ -5781,11 +5736,11 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>324</v>
+      <c r="A14" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>48</v>
@@ -5803,11 +5758,11 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>324</v>
+      <c r="A15" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>48</v>
@@ -5825,11 +5780,11 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>324</v>
+      <c r="A16" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>48</v>
@@ -5847,17 +5802,17 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>324</v>
+      <c r="A17" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>343</v>
+      <c r="D17" s="14">
+        <v>2000.0</v>
       </c>
       <c r="E17" s="1">
         <v>30.0</v>
@@ -5870,7 +5825,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>325</v>
@@ -5892,7 +5847,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>327</v>
@@ -5914,10 +5869,10 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>326</v>
@@ -5936,10 +5891,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>326</v>
@@ -5958,10 +5913,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>326</v>
@@ -5980,10 +5935,10 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>326</v>
@@ -6002,7 +5957,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>325</v>
@@ -6024,7 +5979,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>327</v>
@@ -6046,10 +6001,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>48</v>
@@ -6068,10 +6023,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>351</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>48</v>
@@ -6090,10 +6045,10 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>48</v>
@@ -6112,10 +6067,10 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>48</v>
@@ -6134,10 +6089,10 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>48</v>
@@ -6156,10 +6111,10 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>48</v>
@@ -6178,10 +6133,10 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>48</v>
@@ -6200,10 +6155,10 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>48</v>
@@ -6222,10 +6177,10 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>48</v>
@@ -6244,10 +6199,10 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>48</v>
@@ -6266,10 +6221,10 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>48</v>
@@ -6288,10 +6243,10 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>48</v>
@@ -6310,10 +6265,10 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>48</v>
@@ -6332,10 +6287,10 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>48</v>
@@ -6354,10 +6309,10 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>48</v>
@@ -6376,10 +6331,10 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>48</v>
@@ -6398,10 +6353,10 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>48</v>
@@ -6420,10 +6375,10 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>48</v>
@@ -6442,10 +6397,10 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>48</v>
@@ -6464,10 +6419,10 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>48</v>
@@ -6486,10 +6441,10 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>48</v>
@@ -6508,10 +6463,10 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>48</v>
@@ -6530,10 +6485,10 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>48</v>
@@ -6552,10 +6507,10 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>48</v>
@@ -6574,10 +6529,10 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>48</v>
@@ -6596,10 +6551,10 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>48</v>
@@ -6618,10 +6573,10 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>48</v>
@@ -6640,10 +6595,10 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>48</v>
@@ -6662,10 +6617,10 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>48</v>
@@ -6684,10 +6639,10 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>48</v>
@@ -6704,10 +6659,10 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>48</v>
@@ -6724,10 +6679,10 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>48</v>
@@ -6744,10 +6699,10 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>48</v>
@@ -6764,10 +6719,10 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>48</v>
@@ -6784,10 +6739,10 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>48</v>
@@ -6804,10 +6759,10 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>48</v>
@@ -6824,10 +6779,10 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>48</v>
@@ -6844,10 +6799,10 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>48</v>
@@ -6864,10 +6819,10 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>48</v>
@@ -6884,10 +6839,10 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>48</v>
@@ -6904,10 +6859,10 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>48</v>
@@ -6924,10 +6879,10 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>48</v>
@@ -6944,10 +6899,10 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>48</v>
@@ -6964,10 +6919,10 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>48</v>
@@ -6984,10 +6939,10 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>48</v>
@@ -7004,10 +6959,10 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>48</v>
@@ -7023,8 +6978,8 @@
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="14" t="s">
-        <v>396</v>
+      <c r="A72" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>325</v>
@@ -7043,8 +6998,8 @@
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="14" t="s">
-        <v>396</v>
+      <c r="A73" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>327</v>
@@ -7063,11 +7018,11 @@
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="14" t="s">
-        <v>396</v>
+      <c r="A74" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>48</v>
@@ -7083,11 +7038,11 @@
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="14" t="s">
-        <v>396</v>
+      <c r="A75" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>48</v>
@@ -7103,11 +7058,11 @@
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="14" t="s">
-        <v>396</v>
+      <c r="A76" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>48</v>
@@ -7123,11 +7078,11 @@
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="14" t="s">
-        <v>396</v>
+      <c r="A77" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>48</v>
@@ -7143,11 +7098,11 @@
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="14" t="s">
-        <v>396</v>
+      <c r="A78" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>48</v>
@@ -7163,11 +7118,11 @@
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="14" t="s">
-        <v>396</v>
+      <c r="A79" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>48</v>
@@ -7183,11 +7138,11 @@
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="14" t="s">
-        <v>396</v>
+      <c r="A80" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>48</v>
@@ -7203,11 +7158,11 @@
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="14" t="s">
-        <v>396</v>
+      <c r="A81" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>48</v>
@@ -7223,11 +7178,11 @@
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="14" t="s">
-        <v>396</v>
+      <c r="A82" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>48</v>
@@ -7243,11 +7198,11 @@
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="14" t="s">
-        <v>396</v>
+      <c r="A83" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>48</v>
@@ -7263,11 +7218,11 @@
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="14" t="s">
-        <v>396</v>
+      <c r="A84" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>48</v>
@@ -7283,11 +7238,11 @@
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="14" t="s">
-        <v>396</v>
+      <c r="A85" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>48</v>
@@ -7303,11 +7258,11 @@
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="14" t="s">
-        <v>396</v>
+      <c r="A86" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>48</v>
@@ -7323,11 +7278,11 @@
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="14" t="s">
-        <v>396</v>
+      <c r="A87" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>48</v>
@@ -7343,11 +7298,11 @@
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="14" t="s">
-        <v>396</v>
+      <c r="A88" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>48</v>
@@ -7363,11 +7318,11 @@
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="14" t="s">
-        <v>396</v>
+      <c r="A89" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>48</v>
@@ -7383,11 +7338,11 @@
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="14" t="s">
-        <v>396</v>
+      <c r="A90" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>48</v>
@@ -7403,11 +7358,11 @@
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="14" t="s">
-        <v>396</v>
+      <c r="A91" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>48</v>
@@ -7423,11 +7378,11 @@
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="14" t="s">
-        <v>396</v>
+      <c r="A92" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>48</v>
@@ -7443,11 +7398,11 @@
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="14" t="s">
-        <v>396</v>
+      <c r="A93" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>48</v>
@@ -7463,11 +7418,11 @@
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="14" t="s">
-        <v>396</v>
+      <c r="A94" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>48</v>
@@ -7483,11 +7438,11 @@
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="14" t="s">
-        <v>396</v>
+      <c r="A95" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>48</v>
@@ -7503,11 +7458,11 @@
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="14" t="s">
-        <v>396</v>
+      <c r="A96" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>48</v>
@@ -7523,11 +7478,11 @@
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="14" t="s">
-        <v>396</v>
+      <c r="A97" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>48</v>
@@ -7543,11 +7498,11 @@
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="14" t="s">
-        <v>396</v>
+      <c r="A98" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>48</v>
@@ -7563,11 +7518,11 @@
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="14" t="s">
-        <v>396</v>
+      <c r="A99" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>48</v>
@@ -7583,11 +7538,11 @@
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="14" t="s">
-        <v>396</v>
+      <c r="A100" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>48</v>
@@ -7603,11 +7558,11 @@
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="14" t="s">
-        <v>396</v>
+      <c r="A101" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>48</v>
@@ -7623,11 +7578,11 @@
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="14" t="s">
-        <v>396</v>
+      <c r="A102" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>48</v>
@@ -7643,11 +7598,11 @@
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="14" t="s">
-        <v>396</v>
+      <c r="A103" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>48</v>
@@ -7663,11 +7618,11 @@
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="14" t="s">
-        <v>396</v>
+      <c r="A104" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>48</v>
@@ -7683,11 +7638,11 @@
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="14" t="s">
-        <v>396</v>
+      <c r="A105" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>48</v>
@@ -7703,11 +7658,11 @@
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="14" t="s">
-        <v>396</v>
+      <c r="A106" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>48</v>
@@ -7723,11 +7678,11 @@
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="14" t="s">
-        <v>396</v>
+      <c r="A107" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>48</v>
@@ -7743,11 +7698,11 @@
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="14" t="s">
-        <v>396</v>
+      <c r="A108" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>48</v>
@@ -7763,11 +7718,11 @@
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="14" t="s">
-        <v>396</v>
+      <c r="A109" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>48</v>
@@ -7783,11 +7738,11 @@
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="14" t="s">
-        <v>396</v>
+      <c r="A110" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C110" s="12" t="s">
         <v>48</v>
@@ -7803,11 +7758,11 @@
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="14" t="s">
-        <v>396</v>
+      <c r="A111" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C111" s="12" t="s">
         <v>48</v>
@@ -7823,11 +7778,11 @@
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="14" t="s">
-        <v>396</v>
+      <c r="A112" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>48</v>
@@ -7843,11 +7798,11 @@
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="14" t="s">
-        <v>396</v>
+      <c r="A113" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>48</v>
@@ -7863,11 +7818,11 @@
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="14" t="s">
-        <v>396</v>
+      <c r="A114" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>48</v>
@@ -7883,11 +7838,11 @@
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="14" t="s">
-        <v>396</v>
+      <c r="A115" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>48</v>
@@ -7903,11 +7858,11 @@
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="14" t="s">
-        <v>396</v>
+      <c r="A116" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C116" s="12" t="s">
         <v>48</v>
@@ -7923,11 +7878,11 @@
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="14" t="s">
-        <v>396</v>
+      <c r="A117" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>48</v>
@@ -7943,11 +7898,11 @@
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="14" t="s">
-        <v>396</v>
+      <c r="A118" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>48</v>
@@ -7963,11 +7918,11 @@
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="14" t="s">
-        <v>396</v>
+      <c r="A119" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>48</v>
@@ -7983,11 +7938,11 @@
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="14" t="s">
-        <v>396</v>
+      <c r="A120" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>48</v>
@@ -8003,11 +7958,11 @@
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="14" t="s">
+      <c r="A121" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B121" s="11" t="s">
         <v>396</v>
-      </c>
-      <c r="B121" s="11" t="s">
-        <v>398</v>
       </c>
       <c r="C121" s="12" t="s">
         <v>48</v>
@@ -8023,11 +7978,11 @@
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="14" t="s">
-        <v>396</v>
+      <c r="A122" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C122" s="12" t="s">
         <v>48</v>
@@ -8043,11 +7998,11 @@
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="14" t="s">
-        <v>396</v>
+      <c r="A123" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C123" s="12" t="s">
         <v>48</v>
@@ -8063,11 +8018,11 @@
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="14" t="s">
-        <v>396</v>
+      <c r="A124" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>48</v>
@@ -8083,11 +8038,11 @@
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="14" t="s">
-        <v>396</v>
+      <c r="A125" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>48</v>
@@ -8103,11 +8058,11 @@
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="14" t="s">
-        <v>396</v>
+      <c r="A126" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>48</v>
@@ -8123,11 +8078,11 @@
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="14" t="s">
-        <v>396</v>
+      <c r="A127" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>48</v>
@@ -8143,11 +8098,11 @@
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="14" t="s">
-        <v>396</v>
+      <c r="A128" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>48</v>
@@ -8163,11 +8118,11 @@
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="14" t="s">
-        <v>396</v>
+      <c r="A129" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>48</v>
@@ -8183,11 +8138,11 @@
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="14" t="s">
-        <v>396</v>
+      <c r="A130" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C130" s="12" t="s">
         <v>48</v>
@@ -8203,11 +8158,11 @@
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="14" t="s">
-        <v>396</v>
+      <c r="A131" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>48</v>
@@ -8223,11 +8178,11 @@
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="14" t="s">
-        <v>396</v>
+      <c r="A132" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C132" s="12" t="s">
         <v>48</v>
@@ -8244,10 +8199,10 @@
     </row>
     <row r="133" ht="18.75" customHeight="1">
       <c r="A133" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>326</v>
@@ -8264,10 +8219,10 @@
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="C134" s="12" t="s">
         <v>48</v>
@@ -8284,10 +8239,10 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C135" s="12" t="s">
         <v>48</v>
@@ -8304,10 +8259,10 @@
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C136" s="12" t="s">
         <v>48</v>
@@ -8324,10 +8279,10 @@
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C137" s="12" t="s">
         <v>48</v>
@@ -8344,10 +8299,10 @@
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C138" s="12" t="s">
         <v>48</v>
@@ -8364,10 +8319,10 @@
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>48</v>
@@ -8384,10 +8339,10 @@
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C140" s="12" t="s">
         <v>48</v>
@@ -8404,10 +8359,10 @@
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C141" s="12" t="s">
         <v>48</v>
@@ -8424,10 +8379,10 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>48</v>
@@ -8444,10 +8399,10 @@
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>48</v>
@@ -8464,10 +8419,10 @@
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>48</v>
@@ -8484,10 +8439,10 @@
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>48</v>
@@ -8504,10 +8459,10 @@
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C146" s="12" t="s">
         <v>48</v>
@@ -8524,10 +8479,10 @@
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C147" s="12" t="s">
         <v>48</v>
@@ -8544,10 +8499,10 @@
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>48</v>
@@ -8564,10 +8519,10 @@
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>48</v>
@@ -8584,10 +8539,10 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C150" s="12" t="s">
         <v>48</v>
@@ -8604,10 +8559,10 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>48</v>
@@ -8624,10 +8579,10 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C152" s="12" t="s">
         <v>48</v>
@@ -8644,10 +8599,10 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C153" s="12" t="s">
         <v>48</v>
@@ -8664,10 +8619,10 @@
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C154" s="12" t="s">
         <v>48</v>
@@ -8687,7 +8642,7 @@
         <v>52</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>48</v>
@@ -8707,7 +8662,7 @@
         <v>52</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C156" s="12" t="s">
         <v>48</v>
@@ -8727,7 +8682,7 @@
         <v>52</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C157" s="12" t="s">
         <v>48</v>
@@ -8747,7 +8702,7 @@
         <v>52</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C158" s="12" t="s">
         <v>48</v>
@@ -8767,7 +8722,7 @@
         <v>52</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C159" s="12" t="s">
         <v>48</v>
@@ -8787,13 +8742,13 @@
         <v>52</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C160" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E160" s="1">
         <v>30.0</v>
@@ -8807,7 +8762,7 @@
         <v>52</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>48</v>
@@ -8827,7 +8782,7 @@
         <v>52</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>48</v>
@@ -8847,7 +8802,7 @@
         <v>52</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C163" s="12" t="s">
         <v>48</v>
@@ -8864,7 +8819,7 @@
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>325</v>
@@ -8884,7 +8839,7 @@
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>327</v>
@@ -8904,16 +8859,16 @@
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D166" s="13" t="s">
-        <v>343</v>
+      <c r="D166" s="14">
+        <v>2000.0</v>
       </c>
       <c r="E166" s="1">
         <v>30.0</v>
@@ -8924,16 +8879,16 @@
     </row>
     <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>444</v>
-      </c>
       <c r="C167" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D167" s="13" t="s">
-        <v>445</v>
+      <c r="D167" s="14">
+        <v>1000.0</v>
       </c>
       <c r="E167" s="1">
         <v>30.0</v>
@@ -8944,16 +8899,16 @@
     </row>
     <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C168" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D168" s="13" t="s">
-        <v>343</v>
+      <c r="D168" s="14">
+        <v>2000.0</v>
       </c>
       <c r="E168" s="1">
         <v>30.0</v>
@@ -8964,16 +8919,16 @@
     </row>
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B169" s="11" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C169" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D169" s="13" t="s">
-        <v>448</v>
+      <c r="D169" s="14">
+        <v>10000.0</v>
       </c>
       <c r="E169" s="1">
         <v>30.0</v>
@@ -8984,16 +8939,16 @@
     </row>
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C170" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D170" s="13" t="s">
-        <v>450</v>
+      <c r="D170" s="14">
+        <v>1200.0</v>
       </c>
       <c r="E170" s="1">
         <v>30.0</v>
@@ -9004,16 +8959,16 @@
     </row>
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C171" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D171" s="13" t="s">
-        <v>452</v>
+      <c r="D171" s="14">
+        <v>9000.0</v>
       </c>
       <c r="E171" s="1">
         <v>30.0</v>
@@ -9024,16 +8979,16 @@
     </row>
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C172" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D172" s="13" t="s">
-        <v>335</v>
+      <c r="D172" s="14">
+        <v>5000.0</v>
       </c>
       <c r="E172" s="1">
         <v>30.0</v>
@@ -9044,16 +8999,16 @@
     </row>
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C173" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D173" s="13" t="s">
-        <v>455</v>
+      <c r="D173" s="14">
+        <v>8000.0</v>
       </c>
       <c r="E173" s="1">
         <v>30.0</v>
@@ -9064,16 +9019,16 @@
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C174" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D174" s="13" t="s">
-        <v>455</v>
+      <c r="D174" s="14">
+        <v>8000.0</v>
       </c>
       <c r="E174" s="1">
         <v>30.0</v>
@@ -9084,16 +9039,16 @@
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C175" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D175" s="13" t="s">
-        <v>448</v>
+      <c r="D175" s="14">
+        <v>10000.0</v>
       </c>
       <c r="E175" s="1">
         <v>30.0</v>
@@ -9104,16 +9059,16 @@
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C176" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D176" s="13" t="s">
-        <v>448</v>
+      <c r="D176" s="14">
+        <v>10000.0</v>
       </c>
       <c r="E176" s="1">
         <v>30.0</v>
@@ -9124,16 +9079,16 @@
     </row>
     <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="C177" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D177" s="13" t="s">
-        <v>460</v>
+      <c r="D177" s="14">
+        <v>30000.0</v>
       </c>
       <c r="E177" s="1">
         <v>30.0</v>
@@ -9144,16 +9099,16 @@
     </row>
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="C178" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D178" s="13" t="s">
-        <v>462</v>
+      <c r="D178" s="14">
+        <v>15000.0</v>
       </c>
       <c r="E178" s="1">
         <v>30.0</v>
@@ -9164,16 +9119,16 @@
     </row>
     <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="C179" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D179" s="13" t="s">
-        <v>464</v>
+      <c r="D179" s="14">
+        <v>40000.0</v>
       </c>
       <c r="E179" s="1">
         <v>30.0</v>
@@ -9184,16 +9139,16 @@
     </row>
     <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="C180" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D180" s="13" t="s">
-        <v>466</v>
+      <c r="D180" s="14">
+        <v>12000.0</v>
       </c>
       <c r="E180" s="1">
         <v>30.0</v>
@@ -9204,16 +9159,16 @@
     </row>
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="C181" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D181" s="13" t="s">
-        <v>462</v>
+      <c r="D181" s="14">
+        <v>15000.0</v>
       </c>
       <c r="E181" s="1">
         <v>30.0</v>
@@ -9224,10 +9179,10 @@
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="C182" s="12" t="s">
         <v>48</v>
@@ -9244,16 +9199,16 @@
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="C183" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D183" s="13" t="s">
-        <v>470</v>
+      <c r="D183" s="14">
+        <v>35000.0</v>
       </c>
       <c r="E183" s="1">
         <v>30.0</v>
@@ -9264,16 +9219,16 @@
     </row>
     <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="C184" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D184" s="13" t="s">
-        <v>460</v>
+      <c r="D184" s="14">
+        <v>30000.0</v>
       </c>
       <c r="E184" s="1">
         <v>30.0</v>
@@ -9284,16 +9239,16 @@
     </row>
     <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="C185" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D185" s="13" t="s">
-        <v>464</v>
+      <c r="D185" s="14">
+        <v>40000.0</v>
       </c>
       <c r="E185" s="1">
         <v>30.0</v>
@@ -9304,16 +9259,16 @@
     </row>
     <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="C186" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D186" s="13" t="s">
-        <v>474</v>
+      <c r="D186" s="14">
+        <v>250000.0</v>
       </c>
       <c r="E186" s="1">
         <v>30.0</v>
@@ -9324,16 +9279,16 @@
     </row>
     <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="C187" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D187" s="13" t="s">
-        <v>476</v>
+      <c r="D187" s="14">
+        <v>300000.0</v>
       </c>
       <c r="E187" s="1">
         <v>30.0</v>
@@ -9344,10 +9299,10 @@
     </row>
     <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="C188" s="12" t="s">
         <v>48</v>
@@ -9364,16 +9319,16 @@
     </row>
     <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B189" s="11" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="C189" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D189" s="13" t="s">
-        <v>464</v>
+      <c r="D189" s="14">
+        <v>40000.0</v>
       </c>
       <c r="E189" s="1">
         <v>30.0</v>
@@ -9384,10 +9339,10 @@
     </row>
     <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B190" s="11" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="C190" s="12" t="s">
         <v>48</v>
@@ -9404,10 +9359,10 @@
     </row>
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B191" s="11" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="C191" s="12" t="s">
         <v>48</v>
@@ -9424,10 +9379,10 @@
     </row>
     <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B192" s="11" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="C192" s="12" t="s">
         <v>48</v>
@@ -9444,10 +9399,10 @@
     </row>
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B193" s="11" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="C193" s="12" t="s">
         <v>48</v>
@@ -9464,16 +9419,16 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B194" s="11" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="C194" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D194" s="13" t="s">
-        <v>484</v>
+      <c r="D194" s="14">
+        <v>100000.0</v>
       </c>
       <c r="E194" s="1">
         <v>30.0</v>
@@ -9484,10 +9439,10 @@
     </row>
     <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B195" s="11" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="C195" s="12" t="s">
         <v>48</v>
@@ -9504,16 +9459,16 @@
     </row>
     <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B196" s="11" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="C196" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D196" s="13" t="s">
-        <v>487</v>
+      <c r="D196" s="14">
+        <v>60000.0</v>
       </c>
       <c r="E196" s="1">
         <v>30.0</v>
@@ -9524,16 +9479,16 @@
     </row>
     <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B197" s="11" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="C197" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D197" s="13" t="s">
-        <v>448</v>
+      <c r="D197" s="14">
+        <v>10000.0</v>
       </c>
       <c r="E197" s="1">
         <v>30.0</v>
@@ -9544,16 +9499,16 @@
     </row>
     <row r="198" ht="15.75" customHeight="1">
       <c r="A198" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B198" s="11" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
       <c r="C198" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D198" s="13" t="s">
-        <v>487</v>
+      <c r="D198" s="14">
+        <v>60000.0</v>
       </c>
       <c r="E198" s="1">
         <v>30.0</v>
@@ -9564,16 +9519,16 @@
     </row>
     <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B199" s="11" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="C199" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D199" s="13" t="s">
-        <v>487</v>
+      <c r="D199" s="14">
+        <v>60000.0</v>
       </c>
       <c r="E199" s="1">
         <v>30.0</v>
@@ -9584,7 +9539,7 @@
     </row>
     <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>325</v>
@@ -9604,7 +9559,7 @@
     </row>
     <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>327</v>
@@ -9624,10 +9579,10 @@
     </row>
     <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="C202" s="12" t="s">
         <v>48</v>
@@ -9644,10 +9599,10 @@
     </row>
     <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="C203" s="12" t="s">
         <v>48</v>
@@ -9664,10 +9619,10 @@
     </row>
     <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="C204" s="12" t="s">
         <v>48</v>
@@ -9684,10 +9639,10 @@
     </row>
     <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="C205" s="12" t="s">
         <v>48</v>
@@ -9704,10 +9659,10 @@
     </row>
     <row r="206" ht="15.75" customHeight="1">
       <c r="A206" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="C206" s="12" t="s">
         <v>48</v>
@@ -9724,10 +9679,10 @@
     </row>
     <row r="207" ht="13.5" customHeight="1">
       <c r="A207" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="C207" s="12" t="s">
         <v>48</v>
@@ -9744,10 +9699,10 @@
     </row>
     <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="C208" s="12" t="s">
         <v>48</v>
@@ -9764,10 +9719,10 @@
     </row>
     <row r="209" ht="15.75" customHeight="1">
       <c r="A209" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="C209" s="12" t="s">
         <v>48</v>
@@ -9784,10 +9739,10 @@
     </row>
     <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="C210" s="12" t="s">
         <v>48</v>
@@ -9804,10 +9759,10 @@
     </row>
     <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="C211" s="12" t="s">
         <v>48</v>
@@ -9824,10 +9779,10 @@
     </row>
     <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="C212" s="12" t="s">
         <v>48</v>
@@ -9844,10 +9799,10 @@
     </row>
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="C213" s="12" t="s">
         <v>48</v>
@@ -9864,10 +9819,10 @@
     </row>
     <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="C214" s="12" t="s">
         <v>48</v>
@@ -9884,10 +9839,10 @@
     </row>
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="C215" s="12" t="s">
         <v>48</v>
@@ -9904,10 +9859,10 @@
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="C216" s="12" t="s">
         <v>48</v>
@@ -9924,10 +9879,10 @@
     </row>
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="C217" s="12" t="s">
         <v>48</v>
@@ -9944,10 +9899,10 @@
     </row>
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="C218" s="12" t="s">
         <v>48</v>
@@ -9964,10 +9919,10 @@
     </row>
     <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="C219" s="12" t="s">
         <v>48</v>
@@ -9984,10 +9939,10 @@
     </row>
     <row r="220" ht="15.75" customHeight="1">
       <c r="A220" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="C220" s="12" t="s">
         <v>48</v>
@@ -10004,10 +9959,10 @@
     </row>
     <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="C221" s="12" t="s">
         <v>48</v>
@@ -10024,10 +9979,10 @@
     </row>
     <row r="222" ht="15.75" customHeight="1">
       <c r="A222" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
       <c r="C222" s="12" t="s">
         <v>48</v>
@@ -10044,10 +9999,10 @@
     </row>
     <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="C223" s="12" t="s">
         <v>48</v>
@@ -10064,10 +10019,10 @@
     </row>
     <row r="224" ht="15.75" customHeight="1">
       <c r="A224" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="C224" s="12" t="s">
         <v>48</v>
@@ -10084,10 +10039,10 @@
     </row>
     <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
       <c r="C225" s="12" t="s">
         <v>48</v>
@@ -10104,10 +10059,10 @@
     </row>
     <row r="226" ht="15.75" customHeight="1">
       <c r="A226" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
       <c r="C226" s="12" t="s">
         <v>48</v>
@@ -10124,10 +10079,10 @@
     </row>
     <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="C227" s="12" t="s">
         <v>48</v>
@@ -10144,10 +10099,10 @@
     </row>
     <row r="228" ht="15.75" customHeight="1">
       <c r="A228" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="C228" s="12" t="s">
         <v>48</v>
@@ -10164,10 +10119,10 @@
     </row>
     <row r="229" ht="15.75" customHeight="1">
       <c r="A229" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="C229" s="12" t="s">
         <v>48</v>
@@ -10184,10 +10139,10 @@
     </row>
     <row r="230" ht="15.75" customHeight="1">
       <c r="A230" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="C230" s="12" t="s">
         <v>48</v>
@@ -10204,10 +10159,10 @@
     </row>
     <row r="231" ht="15.75" customHeight="1">
       <c r="A231" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
       <c r="C231" s="12" t="s">
         <v>48</v>
@@ -10224,10 +10179,10 @@
     </row>
     <row r="232" ht="15.75" customHeight="1">
       <c r="A232" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="C232" s="12" t="s">
         <v>48</v>
@@ -10244,10 +10199,10 @@
     </row>
     <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="C233" s="12" t="s">
         <v>48</v>
@@ -10264,10 +10219,10 @@
     </row>
     <row r="234" ht="15.75" customHeight="1">
       <c r="A234" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
       <c r="C234" s="12" t="s">
         <v>48</v>
@@ -10284,10 +10239,10 @@
     </row>
     <row r="235" ht="15.75" customHeight="1">
       <c r="A235" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="C235" s="12" t="s">
         <v>48</v>
@@ -10304,7 +10259,7 @@
     </row>
     <row r="236" ht="15.75" customHeight="1">
       <c r="A236" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>325</v>
@@ -10324,7 +10279,7 @@
     </row>
     <row r="237" ht="15.75" customHeight="1">
       <c r="A237" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>327</v>
@@ -10344,10 +10299,10 @@
     </row>
     <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B238" s="11" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="C238" s="12" t="s">
         <v>48</v>
@@ -10364,10 +10319,10 @@
     </row>
     <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B239" s="11" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="C239" s="12" t="s">
         <v>48</v>
@@ -10384,10 +10339,10 @@
     </row>
     <row r="240" ht="15.75" customHeight="1">
       <c r="A240" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B240" s="11" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="C240" s="12" t="s">
         <v>48</v>
@@ -10404,16 +10359,16 @@
     </row>
     <row r="241" ht="15.75" customHeight="1">
       <c r="A241" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B241" s="11" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="C241" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D241" s="13" t="s">
-        <v>462</v>
+      <c r="D241" s="14">
+        <v>15000.0</v>
       </c>
       <c r="E241" s="1">
         <v>30.0</v>
@@ -10424,10 +10379,10 @@
     </row>
     <row r="242" ht="15.75" customHeight="1">
       <c r="A242" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B242" s="11" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="C242" s="12" t="s">
         <v>48</v>
@@ -10444,10 +10399,10 @@
     </row>
     <row r="243" ht="15.75" customHeight="1">
       <c r="A243" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B243" s="11" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="C243" s="12" t="s">
         <v>48</v>
@@ -10464,16 +10419,16 @@
     </row>
     <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B244" s="11" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="C244" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D244" s="13" t="s">
-        <v>439</v>
+      <c r="D244" s="14">
+        <v>20000.0</v>
       </c>
       <c r="E244" s="1">
         <v>30.0</v>
@@ -10484,10 +10439,10 @@
     </row>
     <row r="245" ht="15.75" customHeight="1">
       <c r="A245" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B245" s="11" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="C245" s="12" t="s">
         <v>48</v>
@@ -10504,10 +10459,10 @@
     </row>
     <row r="246" ht="15.75" customHeight="1">
       <c r="A246" s="12" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B246" s="11" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="C246" s="12" t="s">
         <v>48</v>
@@ -10524,10 +10479,10 @@
     </row>
     <row r="247" ht="15.75" customHeight="1">
       <c r="A247" s="12" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="B247" s="11" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="C247" s="12" t="s">
         <v>48</v>
@@ -10544,10 +10499,10 @@
     </row>
     <row r="248" ht="15.75" customHeight="1">
       <c r="A248" s="12" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="B248" s="11" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
       <c r="C248" s="12" t="s">
         <v>48</v>
@@ -10564,10 +10519,10 @@
     </row>
     <row r="249" ht="15.75" customHeight="1">
       <c r="A249" s="12" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="B249" s="11" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="C249" s="12" t="s">
         <v>48</v>
@@ -10584,10 +10539,10 @@
     </row>
     <row r="250" ht="15.75" customHeight="1">
       <c r="A250" s="12" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="B250" s="11" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="C250" s="12" t="s">
         <v>48</v>

</xml_diff>